<commit_message>
Monitor View Test cases updated
</commit_message>
<xml_diff>
--- a/MMS/Test Cases/MONITOR_VIEW/MONITOR_VIEW1.0.xlsx
+++ b/MMS/Test Cases/MONITOR_VIEW/MONITOR_VIEW1.0.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="120" yWindow="105" windowWidth="20730" windowHeight="9915"/>
@@ -13,12 +13,12 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$5:$I$85</definedName>
   </definedNames>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="149">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="153">
   <si>
     <t>Sl no</t>
   </si>
@@ -421,9 +421,6 @@
 </t>
   </si>
   <si>
-    <t>The alerts or tags or notes should be displayed in the uploaded monitor.</t>
-  </si>
-  <si>
     <t>The alets or tags or notes entered monitor should be updated.</t>
   </si>
   <si>
@@ -745,12 +742,6 @@
     <t>after updating a monitor also it still showing a message "No recent monitor"</t>
   </si>
   <si>
-    <t>Date is displayed as invalid.</t>
-  </si>
-  <si>
-    <t>displays medias  for the selected medias</t>
-  </si>
-  <si>
     <t>it should update monitor with the  "This monitor is not linked to any media  " to "Linked media".</t>
   </si>
   <si>
@@ -773,14 +764,35 @@
     <t>it should update monitor with the "Linked media" to "his monitor is not linked to any media "</t>
   </si>
   <si>
-    <t xml:space="preserve"> month date is not correctLat</t>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>Unable to test</t>
+  </si>
+  <si>
+    <t>all the dates arenot upto date for the range</t>
+  </si>
+  <si>
+    <t>The count of the monitors and in mobile and web is cross verified</t>
+  </si>
+  <si>
+    <t>No monitor images are displayed in shared screen.</t>
+  </si>
+  <si>
+    <t>3G Network the images are not displayed</t>
+  </si>
+  <si>
+    <t>IN THE OFFLINE MODE Date Picker is not working</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> month date is not correctly displayed.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="13" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="13">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1114,14 +1126,14 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1129,49 +1141,7 @@
     <cellStyle name="Excel Built-in Normal" xfId="2"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="9">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="3">
     <dxf>
       <fill>
         <patternFill>
@@ -1278,7 +1248,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -1313,7 +1282,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1489,15 +1457,15 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:I85"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="106" zoomScaleNormal="106" workbookViewId="0">
-      <pane ySplit="5" topLeftCell="A61" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G67" sqref="G67"/>
+      <pane ySplit="5" topLeftCell="A45" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F45" sqref="F45"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="1"/>
     <col min="2" max="2" width="8.7109375" style="1" bestFit="1" customWidth="1"/>
@@ -1510,48 +1478,48 @@
     <col min="9" max="9" width="19.28515625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" ht="15.75" thickBot="1">
       <c r="C1" s="15"/>
-      <c r="D1" s="23" t="s">
-        <v>136</v>
-      </c>
-      <c r="E1" s="24"/>
+      <c r="D1" s="24" t="s">
+        <v>135</v>
+      </c>
+      <c r="E1" s="25"/>
       <c r="F1" s="16"/>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9">
       <c r="C2" s="15"/>
       <c r="D2" s="17" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="E2" s="22">
         <f>COUNTIF(G6:G87, "Pass")</f>
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="F2" s="16"/>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9">
       <c r="C3" s="15"/>
       <c r="D3" s="18" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E3" s="21">
         <f>COUNTIF(G6:G87, "Fail")</f>
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="F3" s="16"/>
     </row>
-    <row r="4" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" ht="15.75" thickBot="1">
       <c r="C4" s="15"/>
       <c r="D4" s="19" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="E4" s="20">
         <f>COUNTIF(G6:G87, "unable to test")</f>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="F4" s="16"/>
     </row>
-    <row r="5" spans="1:9" s="2" customFormat="1" ht="45" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" s="2" customFormat="1" ht="45" customHeight="1" thickTop="1" thickBot="1">
       <c r="A5" s="3" t="s">
         <v>0</v>
       </c>
@@ -1580,7 +1548,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="6" spans="1:9" s="6" customFormat="1" ht="51.75" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9" s="6" customFormat="1" ht="51.75" thickTop="1">
       <c r="A6" s="4">
         <v>1</v>
       </c>
@@ -1600,12 +1568,12 @@
         <v>10</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="H6" s="4"/>
       <c r="I6" s="4"/>
     </row>
-    <row r="7" spans="1:9" s="6" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9" s="6" customFormat="1" ht="51">
       <c r="A7" s="4">
         <v>2</v>
       </c>
@@ -1619,12 +1587,12 @@
         <v>49</v>
       </c>
       <c r="G7" s="4" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="H7" s="4"/>
       <c r="I7" s="4"/>
     </row>
-    <row r="8" spans="1:9" s="6" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9" s="6" customFormat="1" ht="51">
       <c r="A8" s="4">
         <v>3</v>
       </c>
@@ -1638,12 +1606,12 @@
         <v>51</v>
       </c>
       <c r="G8" s="4" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="H8" s="4"/>
       <c r="I8" s="4"/>
     </row>
-    <row r="9" spans="1:9" s="6" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:9" s="6" customFormat="1" ht="51">
       <c r="A9" s="4">
         <v>4</v>
       </c>
@@ -1657,71 +1625,71 @@
         <v>51</v>
       </c>
       <c r="G9" s="4" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="H9" s="4"/>
       <c r="I9" s="4"/>
     </row>
-    <row r="10" spans="1:9" s="6" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:9" s="6" customFormat="1" ht="25.5">
       <c r="A10" s="4">
         <v>5</v>
       </c>
       <c r="B10" s="5"/>
       <c r="C10" s="4"/>
       <c r="D10" s="4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E10" s="4"/>
       <c r="F10" s="12" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="G10" s="4" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="H10" s="4"/>
       <c r="I10" s="4"/>
     </row>
-    <row r="11" spans="1:9" s="6" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" s="6" customFormat="1" ht="30">
       <c r="A11" s="4">
         <v>6</v>
       </c>
       <c r="B11" s="5"/>
       <c r="C11" s="4" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E11" s="4"/>
       <c r="F11" s="4" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="G11" s="4" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="H11" s="4"/>
       <c r="I11" s="4"/>
     </row>
-    <row r="12" spans="1:9" s="6" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" s="6" customFormat="1" ht="30">
       <c r="A12" s="4">
         <v>7</v>
       </c>
       <c r="B12" s="5"/>
       <c r="C12" s="4"/>
       <c r="D12" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E12" s="4"/>
       <c r="F12" s="12" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="G12" s="4" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="H12" s="4"/>
       <c r="I12" s="4"/>
     </row>
-    <row r="13" spans="1:9" s="6" customFormat="1" ht="63.75" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:9" s="6" customFormat="1" ht="63.75">
       <c r="A13" s="4">
         <v>8</v>
       </c>
@@ -1738,17 +1706,17 @@
         <v>12</v>
       </c>
       <c r="F13" s="4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="G13" s="4" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="H13" s="4" t="s">
-        <v>143</v>
+        <v>151</v>
       </c>
       <c r="I13" s="4"/>
     </row>
-    <row r="14" spans="1:9" s="6" customFormat="1" ht="63.75" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:9" s="6" customFormat="1" ht="63.75">
       <c r="A14" s="4">
         <v>9</v>
       </c>
@@ -1763,15 +1731,15 @@
       </c>
       <c r="E14" s="4"/>
       <c r="F14" s="4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G14" s="4" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="H14" s="4"/>
       <c r="I14" s="4"/>
     </row>
-    <row r="15" spans="1:9" s="6" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:9" s="6" customFormat="1" ht="51">
       <c r="A15" s="4">
         <v>10</v>
       </c>
@@ -1786,15 +1754,15 @@
       </c>
       <c r="E15" s="4"/>
       <c r="F15" s="4" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="G15" s="4" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="H15" s="4"/>
       <c r="I15" s="4"/>
     </row>
-    <row r="16" spans="1:9" s="6" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:9" s="6" customFormat="1" ht="51">
       <c r="A16" s="4">
         <v>11</v>
       </c>
@@ -1809,15 +1777,15 @@
       </c>
       <c r="E16" s="4"/>
       <c r="F16" s="4" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="G16" s="4" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="H16" s="4"/>
       <c r="I16" s="4"/>
     </row>
-    <row r="17" spans="1:9" s="6" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:9" s="6" customFormat="1" ht="38.25">
       <c r="A17" s="4">
         <v>12</v>
       </c>
@@ -1835,12 +1803,12 @@
         <v>40</v>
       </c>
       <c r="G17" s="4" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="H17" s="4"/>
       <c r="I17" s="4"/>
     </row>
-    <row r="18" spans="1:9" s="6" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:9" s="6" customFormat="1" ht="38.25">
       <c r="A18" s="4">
         <v>13</v>
       </c>
@@ -1858,12 +1826,12 @@
         <v>39</v>
       </c>
       <c r="G18" s="4" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="H18" s="4"/>
       <c r="I18" s="4"/>
     </row>
-    <row r="19" spans="1:9" s="6" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:9" s="6" customFormat="1" ht="38.25">
       <c r="A19" s="4">
         <v>14</v>
       </c>
@@ -1881,12 +1849,12 @@
         <v>54</v>
       </c>
       <c r="G19" s="4" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="H19" s="4"/>
       <c r="I19" s="4"/>
     </row>
-    <row r="20" spans="1:9" ht="39" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" ht="39">
       <c r="A20" s="4">
         <v>15</v>
       </c>
@@ -1904,12 +1872,12 @@
         <v>38</v>
       </c>
       <c r="G20" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="H20" s="4"/>
       <c r="I20" s="4"/>
     </row>
-    <row r="21" spans="1:9" ht="90" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" ht="90">
       <c r="A21" s="4">
         <v>16</v>
       </c>
@@ -1918,17 +1886,19 @@
       </c>
       <c r="C21" s="4"/>
       <c r="D21" s="4" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E21" s="4"/>
       <c r="F21" s="4" t="s">
-        <v>110</v>
-      </c>
-      <c r="G21" s="4"/>
+        <v>109</v>
+      </c>
+      <c r="G21" s="4" t="s">
+        <v>133</v>
+      </c>
       <c r="H21" s="4"/>
       <c r="I21" s="4"/>
     </row>
-    <row r="22" spans="1:9" ht="90" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" ht="90">
       <c r="A22" s="4">
         <v>17</v>
       </c>
@@ -1943,68 +1913,78 @@
       </c>
       <c r="E22" s="4"/>
       <c r="F22" s="4" t="s">
-        <v>120</v>
-      </c>
-      <c r="G22" s="4"/>
-      <c r="H22" s="4"/>
+        <v>119</v>
+      </c>
+      <c r="G22" s="4" t="s">
+        <v>133</v>
+      </c>
+      <c r="H22" s="4" t="s">
+        <v>148</v>
+      </c>
       <c r="I22" s="4"/>
     </row>
-    <row r="23" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" ht="45">
       <c r="A23" s="4">
         <v>18</v>
       </c>
       <c r="B23" s="5"/>
       <c r="C23" s="4"/>
       <c r="D23" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E23" s="4"/>
       <c r="F23" s="10" t="s">
-        <v>112</v>
-      </c>
-      <c r="G23" s="4"/>
+        <v>111</v>
+      </c>
+      <c r="G23" s="4" t="s">
+        <v>133</v>
+      </c>
       <c r="H23" s="10"/>
       <c r="I23" s="10"/>
     </row>
-    <row r="24" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" ht="45">
       <c r="A24" s="4">
         <v>19</v>
       </c>
       <c r="B24" s="5"/>
       <c r="C24" s="4"/>
       <c r="D24" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E24" s="4"/>
       <c r="F24" s="10" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="G24" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="H24" s="10" t="s">
-        <v>148</v>
+        <v>152</v>
       </c>
       <c r="I24" s="10"/>
     </row>
-    <row r="25" spans="1:9" ht="51.75" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" ht="51.75">
       <c r="A25" s="4">
         <v>20</v>
       </c>
       <c r="B25" s="5"/>
       <c r="C25" s="4"/>
       <c r="D25" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E25" s="4"/>
       <c r="F25" s="10" t="s">
-        <v>113</v>
-      </c>
-      <c r="G25" s="4"/>
-      <c r="H25" s="10"/>
+        <v>112</v>
+      </c>
+      <c r="G25" s="4" t="s">
+        <v>134</v>
+      </c>
+      <c r="H25" s="10" t="s">
+        <v>147</v>
+      </c>
       <c r="I25" s="10"/>
     </row>
-    <row r="26" spans="1:9" s="7" customFormat="1" ht="51.75" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" s="7" customFormat="1" ht="51.75">
       <c r="A26" s="4">
         <v>21</v>
       </c>
@@ -2015,21 +1995,21 @@
         <v>29</v>
       </c>
       <c r="D26" s="4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E26" s="4"/>
       <c r="F26" s="8" t="s">
         <v>30</v>
       </c>
       <c r="G26" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="H26" s="4" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="I26" s="6"/>
     </row>
-    <row r="27" spans="1:9" s="7" customFormat="1" ht="128.25" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" s="7" customFormat="1" ht="128.25">
       <c r="A27" s="4">
         <v>22</v>
       </c>
@@ -2038,57 +2018,59 @@
         <v>36</v>
       </c>
       <c r="D27" s="4" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="E27" s="4"/>
       <c r="F27" s="4" t="s">
-        <v>107</v>
-      </c>
-      <c r="G27" s="4"/>
+        <v>106</v>
+      </c>
+      <c r="G27" s="4" t="s">
+        <v>133</v>
+      </c>
       <c r="H27" s="6"/>
       <c r="I27" s="6"/>
     </row>
-    <row r="28" spans="1:9" s="7" customFormat="1" ht="51.75" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9" s="7" customFormat="1" ht="51.75">
       <c r="A28" s="4">
         <v>23</v>
       </c>
       <c r="B28" s="5"/>
       <c r="C28" s="4"/>
       <c r="D28" s="4" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E28" s="4"/>
       <c r="F28" s="4" t="s">
         <v>37</v>
       </c>
       <c r="G28" s="4" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="H28" s="6"/>
       <c r="I28" s="6"/>
     </row>
-    <row r="29" spans="1:9" s="7" customFormat="1" ht="64.5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9" s="7" customFormat="1" ht="64.5">
       <c r="A29" s="4">
         <v>24</v>
       </c>
       <c r="B29" s="5"/>
       <c r="C29" s="4"/>
       <c r="D29" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E29" s="4"/>
       <c r="F29" s="8" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G29" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="H29" s="4" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="I29" s="6"/>
     </row>
-    <row r="30" spans="1:9" s="7" customFormat="1" ht="39" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9" s="7" customFormat="1" ht="39">
       <c r="A30" s="4">
         <v>25</v>
       </c>
@@ -2101,177 +2083,191 @@
       </c>
       <c r="E30" s="4"/>
       <c r="F30" s="4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G30" s="4" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="H30" s="6"/>
       <c r="I30" s="6"/>
     </row>
-    <row r="31" spans="1:9" s="7" customFormat="1" ht="141" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:9" s="7" customFormat="1" ht="141">
       <c r="A31" s="4">
         <v>26</v>
       </c>
       <c r="B31" s="5"/>
       <c r="C31" s="4"/>
       <c r="D31" s="4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E31" s="4"/>
       <c r="F31" s="10" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="G31" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="H31" s="10" t="s">
-        <v>142</v>
+        <v>150</v>
       </c>
       <c r="I31" s="6"/>
     </row>
-    <row r="32" spans="1:9" s="7" customFormat="1" ht="51.75" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:9" s="7" customFormat="1" ht="51.75">
       <c r="A32" s="4">
         <v>27</v>
       </c>
       <c r="B32" s="5"/>
       <c r="C32" s="4"/>
       <c r="D32" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="F32" s="14" t="s">
         <v>118</v>
-      </c>
-      <c r="F32" s="14" t="s">
-        <v>119</v>
       </c>
       <c r="G32" s="4" t="s">
         <v>134</v>
       </c>
-      <c r="H32" s="6"/>
+      <c r="H32" s="12" t="s">
+        <v>150</v>
+      </c>
       <c r="I32" s="6"/>
     </row>
-    <row r="33" spans="1:9" s="7" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:9" s="7" customFormat="1" ht="60">
       <c r="A33" s="4">
         <v>28</v>
       </c>
       <c r="B33" s="5"/>
       <c r="C33" s="4"/>
       <c r="D33" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E33" s="1"/>
       <c r="F33" s="12" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="G33" s="4" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="H33" s="6"/>
       <c r="I33" s="6"/>
     </row>
-    <row r="34" spans="1:9" s="7" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:9" s="7" customFormat="1" ht="75">
       <c r="A34" s="4">
         <v>29</v>
       </c>
       <c r="B34" s="5"/>
       <c r="C34" s="4"/>
       <c r="D34" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E34" s="1"/>
       <c r="F34" s="12" t="s">
-        <v>85</v>
-      </c>
-      <c r="G34" s="4"/>
-      <c r="H34" s="6"/>
-      <c r="I34" s="6"/>
-    </row>
-    <row r="35" spans="1:9" s="7" customFormat="1" ht="105" x14ac:dyDescent="0.25">
+        <v>84</v>
+      </c>
+      <c r="G34" s="4" t="s">
+        <v>146</v>
+      </c>
+      <c r="H34" s="12" t="s">
+        <v>149</v>
+      </c>
+      <c r="I34" s="12"/>
+    </row>
+    <row r="35" spans="1:9" s="7" customFormat="1" ht="105">
       <c r="A35" s="4">
         <v>30</v>
       </c>
       <c r="B35" s="5"/>
       <c r="C35" s="4"/>
       <c r="D35" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E35" s="1"/>
       <c r="F35" s="12" t="s">
-        <v>88</v>
-      </c>
-      <c r="G35" s="4"/>
+        <v>87</v>
+      </c>
+      <c r="G35" s="4" t="s">
+        <v>146</v>
+      </c>
       <c r="H35" s="6"/>
       <c r="I35" s="6"/>
     </row>
-    <row r="36" spans="1:9" s="7" customFormat="1" ht="105" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:9" s="7" customFormat="1" ht="105">
       <c r="A36" s="4">
         <v>31</v>
       </c>
       <c r="B36" s="5"/>
       <c r="C36" s="4"/>
       <c r="D36" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E36" s="1"/>
       <c r="F36" s="12" t="s">
-        <v>90</v>
-      </c>
-      <c r="G36" s="4"/>
+        <v>89</v>
+      </c>
+      <c r="G36" s="4" t="s">
+        <v>146</v>
+      </c>
       <c r="H36" s="6"/>
       <c r="I36" s="6"/>
     </row>
-    <row r="37" spans="1:9" s="7" customFormat="1" ht="195" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:9" s="7" customFormat="1" ht="195">
       <c r="A37" s="4">
         <v>32</v>
       </c>
       <c r="B37" s="5"/>
       <c r="C37" s="4"/>
       <c r="D37" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E37" s="1"/>
       <c r="F37" s="12" t="s">
-        <v>91</v>
-      </c>
-      <c r="G37" s="4"/>
+        <v>90</v>
+      </c>
+      <c r="G37" s="4" t="s">
+        <v>146</v>
+      </c>
       <c r="H37" s="6"/>
       <c r="I37" s="6"/>
     </row>
-    <row r="38" spans="1:9" s="7" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:9" s="7" customFormat="1" ht="75">
       <c r="A38" s="4">
         <v>33</v>
       </c>
       <c r="B38" s="5"/>
       <c r="C38" s="4"/>
       <c r="D38" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E38" s="1"/>
       <c r="F38" s="12" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="G38" s="4" t="s">
-        <v>134</v>
+        <v>146</v>
       </c>
       <c r="H38" s="6"/>
       <c r="I38" s="6"/>
     </row>
-    <row r="39" spans="1:9" s="7" customFormat="1" ht="105" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:9" s="7" customFormat="1" ht="105">
       <c r="A39" s="4">
         <v>34</v>
       </c>
       <c r="B39" s="5"/>
       <c r="C39" s="4"/>
       <c r="D39" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E39" s="4"/>
       <c r="F39" s="8" t="s">
-        <v>116</v>
-      </c>
-      <c r="G39" s="4"/>
+        <v>115</v>
+      </c>
+      <c r="G39" s="4" t="s">
+        <v>146</v>
+      </c>
       <c r="H39" s="6"/>
       <c r="I39" s="6"/>
     </row>
-    <row r="40" spans="1:9" ht="64.5" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:9" ht="64.5">
       <c r="A40" s="4">
         <v>35</v>
       </c>
@@ -2282,21 +2278,21 @@
         <v>31</v>
       </c>
       <c r="D40" s="4" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E40" s="4"/>
       <c r="F40" s="4" t="s">
         <v>32</v>
       </c>
       <c r="G40" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="H40" s="4" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="I40" s="4"/>
     </row>
-    <row r="41" spans="1:9" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:9" ht="26.25">
       <c r="A41" s="4">
         <v>36</v>
       </c>
@@ -2305,17 +2301,19 @@
       </c>
       <c r="C41" s="4"/>
       <c r="D41" s="4" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E41" s="4"/>
       <c r="F41" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="G41" s="4"/>
+      <c r="G41" s="4" t="s">
+        <v>134</v>
+      </c>
       <c r="H41" s="4"/>
       <c r="I41" s="4"/>
     </row>
-    <row r="42" spans="1:9" ht="51.75" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:9" ht="51.75">
       <c r="A42" s="4">
         <v>37</v>
       </c>
@@ -2324,19 +2322,19 @@
       </c>
       <c r="C42" s="4"/>
       <c r="D42" s="4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E42" s="4"/>
       <c r="F42" s="4" t="s">
         <v>34</v>
       </c>
       <c r="G42" s="4" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="H42" s="4"/>
       <c r="I42" s="4"/>
     </row>
-    <row r="43" spans="1:9" ht="39" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:9" ht="39">
       <c r="A43" s="4">
         <v>38</v>
       </c>
@@ -2345,19 +2343,19 @@
       </c>
       <c r="C43" s="4"/>
       <c r="D43" s="4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E43" s="4"/>
       <c r="F43" s="4" t="s">
         <v>35</v>
       </c>
       <c r="G43" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="H43" s="4"/>
       <c r="I43" s="4"/>
     </row>
-    <row r="44" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:9" ht="30">
       <c r="A44" s="4">
         <v>39</v>
       </c>
@@ -2365,18 +2363,18 @@
         <v>42146</v>
       </c>
       <c r="D44" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="F44" s="12" t="s">
         <v>126</v>
       </c>
-      <c r="F44" s="12" t="s">
-        <v>127</v>
-      </c>
       <c r="G44" s="4" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="H44" s="4"/>
       <c r="I44" s="4"/>
     </row>
-    <row r="45" spans="1:9" ht="153.75" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:9" ht="153.75">
       <c r="A45" s="4">
         <v>40</v>
       </c>
@@ -2385,16 +2383,18 @@
       </c>
       <c r="C45" s="4"/>
       <c r="D45" s="1" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="F45" s="12" t="s">
-        <v>128</v>
-      </c>
-      <c r="G45" s="4"/>
+        <v>127</v>
+      </c>
+      <c r="G45" s="4" t="s">
+        <v>133</v>
+      </c>
       <c r="H45" s="4"/>
       <c r="I45" s="4"/>
     </row>
-    <row r="46" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:9" ht="75">
       <c r="A46" s="4">
         <v>41</v>
       </c>
@@ -2402,18 +2402,18 @@
         <v>42149</v>
       </c>
       <c r="D46" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="F46" s="12" t="s">
         <v>130</v>
       </c>
-      <c r="F46" s="12" t="s">
-        <v>131</v>
-      </c>
       <c r="G46" s="4" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="H46" s="4"/>
       <c r="I46" s="4"/>
     </row>
-    <row r="47" spans="1:9" ht="39" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:9" ht="39">
       <c r="A47" s="4">
         <v>42</v>
       </c>
@@ -2424,19 +2424,19 @@
         <v>42</v>
       </c>
       <c r="D47" s="11" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E47" s="4"/>
       <c r="F47" s="4" t="s">
         <v>43</v>
       </c>
       <c r="G47" s="4" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="H47" s="4"/>
       <c r="I47" s="4"/>
     </row>
-    <row r="48" spans="1:9" ht="39" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:9" ht="39">
       <c r="A48" s="4">
         <v>43</v>
       </c>
@@ -2454,12 +2454,12 @@
         <v>45</v>
       </c>
       <c r="G48" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="H48" s="4"/>
       <c r="I48" s="4"/>
     </row>
-    <row r="49" spans="1:8" ht="39" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:8" ht="39">
       <c r="A49" s="4">
         <v>44</v>
       </c>
@@ -2470,27 +2470,29 @@
         <v>47</v>
       </c>
       <c r="D49" s="4" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="F49" s="12" t="s">
         <v>48</v>
       </c>
-      <c r="G49" s="4"/>
-    </row>
-    <row r="50" spans="1:8" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="G49" s="4" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" ht="26.25">
       <c r="A50" s="4">
         <v>45</v>
       </c>
       <c r="B50" s="5"/>
       <c r="C50" s="4"/>
       <c r="D50" s="4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="G50" s="4" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="51" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" ht="60">
       <c r="A51" s="4">
         <v>46</v>
       </c>
@@ -2501,13 +2503,13 @@
         <v>59</v>
       </c>
       <c r="F51" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="G51" s="25" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="52" spans="1:8" ht="90" x14ac:dyDescent="0.25">
+        <v>123</v>
+      </c>
+      <c r="G51" s="23" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" ht="90">
       <c r="A52" s="4">
         <v>47</v>
       </c>
@@ -2515,16 +2517,16 @@
         <v>42149</v>
       </c>
       <c r="D52" s="9" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="F52" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="G52" s="25" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="53" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="G52" s="23" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" ht="45">
       <c r="A53" s="4">
         <v>48</v>
       </c>
@@ -2537,11 +2539,11 @@
       <c r="F53" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="G53" s="25" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="54" spans="1:8" ht="105" x14ac:dyDescent="0.25">
+      <c r="G53" s="23" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" ht="105">
       <c r="A54" s="4">
         <v>49</v>
       </c>
@@ -2551,12 +2553,14 @@
       <c r="D54" s="9" t="s">
         <v>63</v>
       </c>
-      <c r="F54" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="G54" s="25"/>
-    </row>
-    <row r="55" spans="1:8" ht="165" x14ac:dyDescent="0.25">
+      <c r="F54" s="9" t="s">
+        <v>145</v>
+      </c>
+      <c r="G54" s="23" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8" ht="165">
       <c r="A55" s="4">
         <v>50</v>
       </c>
@@ -2564,34 +2568,34 @@
         <v>42149</v>
       </c>
       <c r="D55" s="9" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F55" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="G55" s="25" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="56" spans="1:8" ht="120" x14ac:dyDescent="0.25">
+        <v>64</v>
+      </c>
+      <c r="G55" s="23" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8" ht="120">
       <c r="A56" s="4">
         <v>51</v>
       </c>
       <c r="B56" s="5"/>
       <c r="D56" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="F56" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="F56" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="G56" s="25" t="s">
-        <v>134</v>
+      <c r="G56" s="23" t="s">
+        <v>133</v>
       </c>
       <c r="H56" s="1" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="57" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8" ht="60">
       <c r="A57" s="4">
         <v>52</v>
       </c>
@@ -2599,16 +2603,16 @@
         <v>42149</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="F57" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="G57" s="25" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="58" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+        <v>79</v>
+      </c>
+      <c r="G57" s="23" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8" ht="60">
       <c r="A58" s="4">
         <v>53</v>
       </c>
@@ -2616,16 +2620,16 @@
         <v>42149</v>
       </c>
       <c r="D58" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="F58" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="F58" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="G58" s="25" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="59" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="G58" s="23" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8" ht="45">
       <c r="A59" s="4">
         <v>54</v>
       </c>
@@ -2633,13 +2637,13 @@
         <v>42149</v>
       </c>
       <c r="F59" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="G59" s="25" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="60" spans="1:8" ht="165" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+      <c r="G59" s="23" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8" ht="165">
       <c r="A60" s="4">
         <v>55</v>
       </c>
@@ -2647,16 +2651,16 @@
         <v>42149</v>
       </c>
       <c r="D60" s="1" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="F60" s="1" t="s">
-        <v>144</v>
-      </c>
-      <c r="G60" s="25" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="61" spans="1:8" ht="165" x14ac:dyDescent="0.25">
+        <v>141</v>
+      </c>
+      <c r="G60" s="23" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8" ht="165">
       <c r="A61" s="4">
         <v>56</v>
       </c>
@@ -2664,16 +2668,16 @@
         <v>42149</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="F61" s="1" t="s">
-        <v>147</v>
-      </c>
-      <c r="G61" s="25" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
+        <v>144</v>
+      </c>
+      <c r="G61" s="23" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="62" spans="1:8">
       <c r="A62" s="4">
         <v>57</v>
       </c>
@@ -2681,7 +2685,7 @@
         <v>42149</v>
       </c>
     </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:8">
       <c r="A63" s="4">
         <v>58</v>
       </c>
@@ -2689,7 +2693,7 @@
         <v>42149</v>
       </c>
     </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:8">
       <c r="A64" s="4">
         <v>59</v>
       </c>
@@ -2697,7 +2701,7 @@
         <v>42149</v>
       </c>
     </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:2">
       <c r="A65" s="4">
         <v>60</v>
       </c>
@@ -2705,7 +2709,7 @@
         <v>42149</v>
       </c>
     </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:2">
       <c r="A66" s="4">
         <v>61</v>
       </c>
@@ -2713,7 +2717,7 @@
         <v>42149</v>
       </c>
     </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:2">
       <c r="A67" s="4">
         <v>62</v>
       </c>
@@ -2721,7 +2725,7 @@
         <v>42149</v>
       </c>
     </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:2">
       <c r="A68" s="4">
         <v>63</v>
       </c>
@@ -2729,7 +2733,7 @@
         <v>42149</v>
       </c>
     </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:2">
       <c r="A69" s="4">
         <v>64</v>
       </c>
@@ -2737,7 +2741,7 @@
         <v>42149</v>
       </c>
     </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:2">
       <c r="A70" s="4">
         <v>65</v>
       </c>
@@ -2745,7 +2749,7 @@
         <v>42149</v>
       </c>
     </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:2">
       <c r="A71" s="4">
         <v>66</v>
       </c>
@@ -2753,7 +2757,7 @@
         <v>42149</v>
       </c>
     </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:2">
       <c r="A72" s="4">
         <v>67</v>
       </c>
@@ -2761,7 +2765,7 @@
         <v>42149</v>
       </c>
     </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:2">
       <c r="A73" s="4">
         <v>68</v>
       </c>
@@ -2769,7 +2773,7 @@
         <v>42149</v>
       </c>
     </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:2">
       <c r="A74" s="4">
         <v>69</v>
       </c>
@@ -2777,57 +2781,57 @@
         <v>42149</v>
       </c>
     </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:2">
       <c r="A75" s="4">
         <v>70</v>
       </c>
     </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:2">
       <c r="A76" s="4">
         <v>71</v>
       </c>
     </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:2">
       <c r="A77" s="4">
         <v>72</v>
       </c>
     </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:2">
       <c r="A78" s="4">
         <v>73</v>
       </c>
     </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:2">
       <c r="A79" s="4">
         <v>74</v>
       </c>
     </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:2">
       <c r="A80" s="4">
         <v>75</v>
       </c>
     </row>
-    <row r="81" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:1">
       <c r="A81" s="4">
         <v>76</v>
       </c>
     </row>
-    <row r="82" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:1">
       <c r="A82" s="4">
         <v>77</v>
       </c>
     </row>
-    <row r="83" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:1">
       <c r="A83" s="4">
         <v>78</v>
       </c>
     </row>
-    <row r="84" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:1">
       <c r="A84" s="4">
         <v>79</v>
       </c>
     </row>
-    <row r="85" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:1">
       <c r="A85" s="4">
         <v>80</v>
       </c>
@@ -2838,13 +2842,13 @@
     <mergeCell ref="D1:E1"/>
   </mergeCells>
   <conditionalFormatting sqref="G6:G61">
-    <cfRule type="cellIs" dxfId="8" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
       <formula>"Unable to test"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
       <formula>"fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="3" operator="equal">
       <formula>"pass"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2859,12 +2863,12 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>